<commit_message>
% AS coverage code and it's results are added
</commit_message>
<xml_diff>
--- a/heavy_hitter_AS/parent_child_time_execution_analysis.xlsx
+++ b/heavy_hitter_AS/parent_child_time_execution_analysis.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>Parent number</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>as_relationship_graph.txt</t>
+  </si>
+  <si>
+    <t>5888(with% Ases covered part)</t>
   </si>
   <si>
     <t>countries/south_korea.html</t>
@@ -223,21 +226,21 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$16</c:f>
+              <c:f>Sheet1!$A$2:$A$17</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$16</c:f>
+              <c:f>Sheet1!$B$2:$B$17</c:f>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1353698122"/>
-        <c:axId val="990026844"/>
+        <c:axId val="1175565754"/>
+        <c:axId val="330201512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1353698122"/>
+        <c:axId val="1175565754"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -282,10 +285,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="990026844"/>
+        <c:crossAx val="330201512"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="990026844"/>
+        <c:axId val="330201512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -354,7 +357,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1353698122"/>
+        <c:crossAx val="1175565754"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -833,28 +836,34 @@
       </c>
     </row>
     <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="D17" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18">
       <c r="D18" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19">
       <c r="D19" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>